<commit_message>
Se crea metodo para comprobar si existe el archivo basura, y para comprobar si existe el folder de los archivos nuevos renombrados temporalmente, metodo para renombrar temporalemente el archivo ubicar en folder, metodo para renombrar todos los archivos en el folder y metodo que ordena la lista de metadatos por fecha
</commit_message>
<xml_diff>
--- a/generated_files/0_0ReadData.xlsx
+++ b/generated_files/0_0ReadData.xlsx
@@ -14,45 +14,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>003_ESCRITO_DEMANDA_FLS._1-73.pdf</t>
-  </si>
-  <si>
-    <t>009 2020 - 133 OFICIO EPS (Fl. 40).pdf</t>
-  </si>
-  <si>
-    <t>002 ACTA DE REPARTO.pdf</t>
-  </si>
-  <si>
-    <t>001 CARATULA.pdf</t>
-  </si>
-  <si>
-    <t>004 2020-566 AUTO LIBRA MANDAMIENTO HIPOTECARIO (FLS. 74-76).pdf</t>
-  </si>
-  <si>
-    <t>005 2020-566 OFICIO INSCRIPCION EMBARGO INMUEBLE (FLS. 77-78).pdf</t>
-  </si>
-  <si>
-    <t>006 2020-566  SOLICITUD DE CORRECCIÓN DE AUTO (FLS. 79-80).pdf</t>
-  </si>
-  <si>
-    <t>007 2020-566 AUTO CORRIGE ERROR (FLS. 81-83).pdf</t>
-  </si>
-  <si>
-    <t>008 2020-566 CONSTANCIA DE ENTREGA (17 DE FEBRERO).pdf</t>
-  </si>
-  <si>
-    <t>009 2020-566 ENVIO Y ENTREGA D ENOTIFICACIÓN PERSONAL (FLS. 85-88).pdf</t>
-  </si>
-  <si>
-    <t>004 2020-107 OFICIO LEVANTA EMBARGO VEHICULO (FLS. 37-38).pdf</t>
-  </si>
-  <si>
-    <t>010 2020-566 AUTO OSA HIPOTECARIO DECRETO (FLS. 89-93).pdf</t>
-  </si>
-  <si>
-    <t>011 2020-566 CONSTANCIA DE ENTREGA AUTO (05 DE ABRIL).pdf</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>01._CARATULA.pdf</t>
+  </si>
+  <si>
+    <t>03._aUTO_ADMITE_demaNDA.pdf</t>
+  </si>
+  <si>
+    <t>02._acta_de_reparto.pdf</t>
+  </si>
+  <si>
+    <t>04._MEMORIAL.pdf</t>
+  </si>
+  <si>
+    <t>05._CONSTANCIA_21-03-2021.pdf</t>
+  </si>
+  <si>
+    <t>06._notificación_19.04.2021_DEMANDADO.pdf</t>
+  </si>
+  <si>
+    <t>07._MEMORIAL,_NO_ACEPTA_DESIGNACION.pdf</t>
+  </si>
+  <si>
+    <t>08._AUTO_NOMBRA_CURADOR.pdf</t>
+  </si>
+  <si>
+    <t>09._acuse_recibido.pdf</t>
+  </si>
+  <si>
+    <t>10._AcEpTa_dEsIgNaCióN.pdf</t>
+  </si>
+  <si>
+    <t>11._NOTIFICACION._CURADOR..pdf</t>
+  </si>
+  <si>
+    <t>12._CONSTESTACION_CURADOR_AD_LITEM.pdf</t>
+  </si>
+  <si>
+    <t>13._MEMORIAL-SOLICITUD-CELERIDAD.pdf</t>
+  </si>
+  <si>
+    <t>14._AUTO-ORDENA--SEGUIR...ADELANTE-EJECUCION.pdf</t>
   </si>
 </sst>
 </file>
@@ -388,7 +391,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -396,10 +399,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1">
-        <v>44037</v>
+        <v>43999.37777777778</v>
       </c>
       <c r="B1">
-        <v>73</v>
+        <v>115</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -407,10 +410,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1">
-        <v>44165.72513888889</v>
+        <v>44064.87149305556</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -418,10 +421,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1">
-        <v>44183</v>
+        <v>44064.87149305556</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -429,10 +432,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1">
-        <v>44183.4015162037</v>
+        <v>44123.48692129629</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -440,7 +443,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1">
-        <v>44228.53858796296</v>
+        <v>44138.73788194444</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -451,10 +454,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1">
-        <v>44228.60296296296</v>
+        <v>44146.6043287037</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -462,10 +465,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1">
-        <v>44235</v>
+        <v>44148.70625</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -473,7 +476,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1">
-        <v>44243.61565972222</v>
+        <v>44169.64605324074</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -484,7 +487,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1">
-        <v>44244.54597222222</v>
+        <v>44181.51538194445</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -495,10 +498,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1">
-        <v>44265</v>
+        <v>44184</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
@@ -506,7 +509,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1">
-        <v>44272.61548611111</v>
+        <v>44214</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -517,10 +520,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1">
-        <v>44281.54908564815</v>
+        <v>44228</v>
       </c>
       <c r="B12">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
@@ -528,13 +531,24 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1">
-        <v>44291.56090277778</v>
+        <v>44231</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1">
+        <v>44246.64069444445</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agrego script para elimina la carpeta de los nuevos archivos en caso de existir, se descomenta codigo que hace el cambio de nombre y se crea metodo que ordena la lista list_metadata_dates
</commit_message>
<xml_diff>
--- a/generated_files/0_0ReadData.xlsx
+++ b/generated_files/0_0ReadData.xlsx
@@ -16,46 +16,46 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
-    <t>01._CARATULA.pdf</t>
-  </si>
-  <si>
-    <t>03._aUTO_ADMITE_demaNDA.pdf</t>
-  </si>
-  <si>
-    <t>02._acta_de_reparto.pdf</t>
-  </si>
-  <si>
-    <t>04._MEMORIAL.pdf</t>
-  </si>
-  <si>
-    <t>05._CONSTANCIA_21-03-2021.pdf</t>
-  </si>
-  <si>
-    <t>06._notificación_19.04.2021_DEMANDADO.pdf</t>
-  </si>
-  <si>
-    <t>07._MEMORIAL,_NO_ACEPTA_DESIGNACION.pdf</t>
-  </si>
-  <si>
-    <t>08._AUTO_NOMBRA_CURADOR.pdf</t>
-  </si>
-  <si>
-    <t>09._acuse_recibido.pdf</t>
-  </si>
-  <si>
-    <t>10._AcEpTa_dEsIgNaCióN.pdf</t>
-  </si>
-  <si>
-    <t>11._NOTIFICACION._CURADOR..pdf</t>
-  </si>
-  <si>
-    <t>12._CONSTESTACION_CURADOR_AD_LITEM.pdf</t>
-  </si>
-  <si>
-    <t>13._MEMORIAL-SOLICITUD-CELERIDAD.pdf</t>
-  </si>
-  <si>
-    <t>14._AUTO-ORDENA--SEGUIR...ADELANTE-EJECUCION.pdf</t>
+    <t>01Caratula.pdf</t>
+  </si>
+  <si>
+    <t>02AutoAdmiteDemanda.pdf</t>
+  </si>
+  <si>
+    <t>03ActaDeReparto.pdf</t>
+  </si>
+  <si>
+    <t>04Memorial.pdf</t>
+  </si>
+  <si>
+    <t>05Constancia20210321.pdf</t>
+  </si>
+  <si>
+    <t>06NotificacionDemandado.pdf</t>
+  </si>
+  <si>
+    <t>07MemorialNoAceptaDesignacion.pdf</t>
+  </si>
+  <si>
+    <t>08AutoNombraCurador.pdf</t>
+  </si>
+  <si>
+    <t>09AcuseRecibido.pdf</t>
+  </si>
+  <si>
+    <t>10AceptaDesignacion.pdf</t>
+  </si>
+  <si>
+    <t>11NotificacionCurador.pdf</t>
+  </si>
+  <si>
+    <t>12ConstestacionCuradorAdLitem.pdf</t>
+  </si>
+  <si>
+    <t>13MemorialSolicitudCeleridad.pdf</t>
+  </si>
+  <si>
+    <t>14AutoOrdenaSeguirAdelanteEjecucion.pdf</t>
   </si>
 </sst>
 </file>

</xml_diff>